<commit_message>
Strengthening the crosswalk to create our AICM database
</commit_message>
<xml_diff>
--- a/book/DATA/AICM_Cognates_Master.xlsx
+++ b/book/DATA/AICM_Cognates_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\aimoralcode-core\book\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4A5104C-200C-49C3-8CE3-E6F4AB9698BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19ABD8C-E26F-4A7F-B37F-6A37F3D99372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13634,7 +13634,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13943,7 +13943,7 @@
   <dimension ref="A1:AE272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F160" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1"/>
@@ -13955,7 +13955,9 @@
     <col min="6" max="6" width="175.33203125" style="14" customWidth="1"/>
     <col min="7" max="11" width="20.77734375" customWidth="1"/>
     <col min="12" max="12" width="82.44140625" style="3" customWidth="1"/>
-    <col min="13" max="27" width="20.77734375" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" customWidth="1"/>
+    <col min="14" max="14" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="27" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.95" customHeight="1">

</xml_diff>